<commit_message>
some bugs fixed to perform the multiplications
</commit_message>
<xml_diff>
--- a/src/main/resources/out/performance_metrics_parallel.xlsx
+++ b/src/main/resources/out/performance_metrics_parallel.xlsx
@@ -12,10 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Matrix Generation Time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Parallel Multiplication Time</t>
   </si>
@@ -62,7 +59,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -73,15 +70,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="n" s="0">
-        <v>3.26E-5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>0.0022951</v>
+        <v>0.0300042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>